<commit_message>
Ejemplo de emprimir fila completa
</commit_message>
<xml_diff>
--- a/hello world.xlsx
+++ b/hello world.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projects\hola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5080644F-25ED-47FA-8B94-BEDE01DA4483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C21781-6874-41B4-8ECB-AF9A11A14BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -413,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,9 +473,6 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H8" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G15" s="1"/>
-    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -487,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECE52F02-6421-4ADA-ADE8-9F518D02CA27}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A1:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>